<commit_message>
UPDATE[calc]: All the engineering functions (#238)
54 new functions!

This includes:

* Number basis functions. To convert back and forth from different
  number basis (12 functions)
* Bit functions. To perform bitwise operations with numbers (5 functions)
* Complex functions, to do arithmetic and trigonometry
  with complex numbers (26 functions)
* Bessel functions and error functions (8 functions)
* CONVERT function to convert measurements from and back many units
* DELTA and GESTEP functions
</commit_message>
<xml_diff>
--- a/packages/calc/equalto_xlsx/tests/calc_tests/IRR.xlsx
+++ b/packages/calc/equalto_xlsx/tests/calc_tests/IRR.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DC7655-4A9C-8447-B570-99BEB0949643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2A0B81-E134-8B40-8F1A-A3317686D08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{A0705745-E7DF-B343-9A23-E8010C92D60D}"/>
+    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{A0705745-E7DF-B343-9A23-E8010C92D60D}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Two Values" sheetId="2" r:id="rId2"/>
     <sheet name="Three Parameters" sheetId="3" r:id="rId3"/>
+    <sheet name="METADATA" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -194,7 +195,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
@@ -206,6 +207,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -524,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF106676-309E-3143-B823-36DD99969B65}">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
@@ -2398,4 +2400,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A86C73E-B491-D14F-95E3-0838E2BC1E45}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11">
+        <v>4.9999999999999998E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>